<commit_message>
Aggiornato file excelper casi di OK
Aggiornati riferimenti per casi di OK (450, 451)
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111DELTAINFORMATICASRLXX/Delta_Informatica_srl/MYSANITA_LDO/25/report-checklist-LDO_V8.2.6.1_MYSANITA_LDO.xlsx
+++ b/GATEWAY/A1#111DELTAINFORMATICASRLXX/Delta_Informatica_srl/MYSANITA_LDO/25/report-checklist-LDO_V8.2.6.1_MYSANITA_LDO.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29518"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\irene.stacchiotti\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{37473C85-A5C9-4CEC-A80D-6ADA9FE5C972}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{678A7490-5354-4AD1-B50B-3A92AC7C08B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="33720" yWindow="975" windowWidth="29040" windowHeight="15720" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -585,16 +585,16 @@
 Il Documento CDA2 Lettera Dimissione Ospedaliera dovrà essere composto in modo da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 17" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>14/11/2025</t>
-  </si>
-  <si>
-    <t>2025-11-14T17:25:30Z</t>
-  </si>
-  <si>
-    <t>db0fe3d09700d6078bd04d36e503b06c</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.30.4.4.eb54817f525019dc3de6a95f43b03d53d017aaf12e33863a9c932a978f19c2ff.3e17a7e921^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>21/11/2025</t>
+  </si>
+  <si>
+    <t>2025-11-21T09:39:57Z</t>
+  </si>
+  <si>
+    <t>d1788bff196d93684dee813a5e763f19</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.30.4.4.eb54817f525019dc3de6a95f43b03d53d017aaf12e33863a9c932a978f19c2ff.7de2237f1e^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>OK</t>
@@ -607,13 +607,13 @@
 Il Documento CDA2 Lettera Dimissione Ospedaliera dovrà essere composto in modo da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 18" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2025-11-14T17:32:05Z</t>
-  </si>
-  <si>
-    <t>5c05642501243b9cbf15a757f0b42abf</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.30.4.4.eb54817f525019dc3de6a95f43b03d53d017aaf12e33863a9c932a978f19c2ff.e3906d84c8^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2025-11-21T10:43:39Z</t>
+  </si>
+  <si>
+    <t>25f3b2ea8cd65ea6286205263afb6a85</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.30.4.4.eb54817f525019dc3de6a95f43b03d53d017aaf12e33863a9c932a978f19c2ff.9f4ef2ee81^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_LDO_CT19_KO</t>
@@ -2834,8 +2834,8 @@
   <dimension ref="A1:W580"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="9" topLeftCell="E23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F24" sqref="F24"/>
+      <pane ySplit="9" topLeftCell="D21" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I24" sqref="I24"/>
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
@@ -10308,6 +10308,27 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <UserStoryALM xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A92AB09DCDF6014AA0D6826BF29E2C8E" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d4db60622090a1f8a8d506ac1d64a349">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1e76d14e-d0ce-457c-8343-9b55836d9ead" xmlns:ns3="a56712a3-8dfd-4688-917a-22f0cf513b89" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0a3a9ed8bb952a3d76dd1e2fa3d624b9" ns2:_="" ns3:_="">
     <xsd:import namespace="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
@@ -10565,29 +10586,8 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <UserStoryALM xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ACB08642-5694-4F88-BF6F-98521E3A5E0B}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4C806F-EC4E-4231-9462-6D32094C4603}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -10595,7 +10595,7 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4C806F-EC4E-4231-9462-6D32094C4603}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ACB08642-5694-4F88-BF6F-98521E3A5E0B}"/>
 </file>
 
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>